<commit_message>
put some cards from cube to edh
</commit_message>
<xml_diff>
--- a/cube_cards.xlsx
+++ b/cube_cards.xlsx
@@ -5316,10 +5316,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -5345,7 +5345,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5353,7 +5353,43 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5374,8 +5410,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5386,6 +5431,30 @@
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -5404,75 +5473,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -5489,7 +5489,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5501,13 +5609,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5525,72 +5657,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -5598,72 +5664,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5692,21 +5692,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -5716,11 +5701,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5732,15 +5732,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5761,16 +5752,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5780,10 +5780,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -5792,130 +5792,130 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -6246,8 +6246,8 @@
   <sheetPr/>
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="D171" workbookViewId="0">
+      <selection activeCell="N171" sqref="N171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -13772,7 +13772,7 @@
         <v>0</v>
       </c>
       <c r="N171">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:14">
@@ -22862,7 +22862,7 @@
         <v>0</v>
       </c>
       <c r="N378">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="379" spans="1:14">
@@ -38617,7 +38617,7 @@
         <v>0</v>
       </c>
       <c r="N739">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="740" spans="1:14">
@@ -49000,7 +49000,7 @@
         <v>0</v>
       </c>
       <c r="N979">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="980" spans="1:14">
@@ -49082,7 +49082,7 @@
         <v>0</v>
       </c>
       <c r="N981">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="982" spans="1:14">

</xml_diff>

<commit_message>
buy Talismans and Signets
</commit_message>
<xml_diff>
--- a/cube_cards.xlsx
+++ b/cube_cards.xlsx
@@ -5317,9 +5317,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -5337,82 +5337,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -5445,14 +5369,60 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5473,6 +5443,36 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -5483,13 +5483,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5507,7 +5627,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5519,151 +5663,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5677,32 +5677,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5757,11 +5736,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5780,10 +5780,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -5792,133 +5792,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -34058,7 +34058,7 @@
         <v>0</v>
       </c>
       <c r="N633">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="634" spans="1:14">
@@ -34102,7 +34102,7 @@
         <v>0</v>
       </c>
       <c r="N634">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="635" spans="1:14">
@@ -34920,7 +34920,7 @@
         <v>0</v>
       </c>
       <c r="N653">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="654" spans="1:14">
@@ -34964,7 +34964,7 @@
         <v>0</v>
       </c>
       <c r="N654">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="655" spans="1:14">
@@ -35691,7 +35691,7 @@
         <v>0</v>
       </c>
       <c r="N671">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="672" spans="1:14">
@@ -35735,7 +35735,7 @@
         <v>0</v>
       </c>
       <c r="N672">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="673" spans="1:14">
@@ -36509,7 +36509,7 @@
         <v>0</v>
       </c>
       <c r="N690">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="691" spans="1:14">
@@ -36553,7 +36553,7 @@
         <v>0</v>
       </c>
       <c r="N691">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="692" spans="1:14">
@@ -37456,7 +37456,7 @@
         <v>0</v>
       </c>
       <c r="N712">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="713" spans="1:14">
@@ -37500,7 +37500,7 @@
         <v>0</v>
       </c>
       <c r="N713">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="714" spans="1:14">
@@ -38576,7 +38576,7 @@
         <v>0</v>
       </c>
       <c r="N738">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="739" spans="1:14">
@@ -39523,7 +39523,7 @@
         <v>0</v>
       </c>
       <c r="N760">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="761" spans="1:14">
@@ -40514,7 +40514,7 @@
         <v>0</v>
       </c>
       <c r="N783">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="784" spans="1:14">
@@ -41373,7 +41373,7 @@
         <v>0</v>
       </c>
       <c r="N803">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="804" spans="1:14">
@@ -42232,7 +42232,7 @@
         <v>0</v>
       </c>
       <c r="N823">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="824" spans="1:14">

</xml_diff>

<commit_message>
buy a bunch of cards
</commit_message>
<xml_diff>
--- a/cube_cards.xlsx
+++ b/cube_cards.xlsx
@@ -5041,9 +5041,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -5062,23 +5062,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -5089,9 +5083,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5105,33 +5098,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5145,13 +5120,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -5160,23 +5128,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF0000FF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5197,6 +5151,52 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -5207,31 +5207,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5255,13 +5237,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5279,7 +5267,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5291,25 +5291,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5321,31 +5315,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5363,31 +5333,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5398,6 +5398,69 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -5422,30 +5485,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -5459,55 +5498,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -5516,133 +5516,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -6339,7 +6339,7 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -11610,7 +11610,7 @@
         <v>0</v>
       </c>
       <c r="N128">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:14">
@@ -12094,7 +12094,7 @@
         <v>0</v>
       </c>
       <c r="N139">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:14">
@@ -12487,7 +12487,7 @@
         <v>1</v>
       </c>
       <c r="N148">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:14">
@@ -12619,7 +12619,7 @@
         <v>1</v>
       </c>
       <c r="N151">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:14">
@@ -12924,7 +12924,7 @@
         <v>0</v>
       </c>
       <c r="N158">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:14">
@@ -17353,7 +17353,7 @@
         <v>1</v>
       </c>
       <c r="N259">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="260" spans="1:14">
@@ -24120,7 +24120,7 @@
         <v>0</v>
       </c>
       <c r="N413">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="414" spans="1:14">
@@ -25308,7 +25308,7 @@
         <v>0</v>
       </c>
       <c r="N440">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="441" spans="1:14">
@@ -25924,7 +25924,7 @@
         <v>0</v>
       </c>
       <c r="N454">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="455" spans="1:14">
@@ -26713,7 +26713,7 @@
         <v>0</v>
       </c>
       <c r="N472">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="473" spans="1:14">
@@ -27285,7 +27285,7 @@
         <v>1</v>
       </c>
       <c r="N485">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="486" spans="1:14">
@@ -30664,7 +30664,7 @@
         <v>0</v>
       </c>
       <c r="N562">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="563" spans="1:14">
@@ -31280,7 +31280,7 @@
         <v>0</v>
       </c>
       <c r="N576">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="577" spans="1:14">
@@ -32142,7 +32142,7 @@
         <v>0</v>
       </c>
       <c r="N596">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="597" spans="1:14">
@@ -35282,7 +35282,7 @@
         <v>0</v>
       </c>
       <c r="N669">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="670" spans="1:14">
@@ -36572,7 +36572,7 @@
         <v>0</v>
       </c>
       <c r="N699">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="700" spans="1:14">
@@ -38375,7 +38375,7 @@
         <v>0</v>
       </c>
       <c r="N741">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="742" spans="1:14">
@@ -39149,7 +39149,7 @@
         <v>0</v>
       </c>
       <c r="N759">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="760" spans="1:14">
@@ -39190,7 +39190,7 @@
         <v>0</v>
       </c>
       <c r="N760">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="761" spans="1:14">
@@ -40310,7 +40310,7 @@
         <v>0</v>
       </c>
       <c r="N786">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="787" spans="1:14">
@@ -40524,7 +40524,7 @@
         <v>0</v>
       </c>
       <c r="N791">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="792" spans="1:14">
@@ -40826,7 +40826,7 @@
         <v>0</v>
       </c>
       <c r="N798">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="799" spans="1:14">
@@ -42234,7 +42234,7 @@
         <v>0</v>
       </c>
       <c r="N830">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="831" spans="1:14">
@@ -42806,7 +42806,7 @@
         <v>1</v>
       </c>
       <c r="N843">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="844" spans="1:14">
@@ -44915,7 +44915,7 @@
         <v>0</v>
       </c>
       <c r="N891">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="892" spans="1:14">
@@ -45492,7 +45492,7 @@
         <v>0</v>
       </c>
       <c r="N905">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="906" spans="1:14">
@@ -45656,7 +45656,7 @@
         <v>0</v>
       </c>
       <c r="N909">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="910" spans="1:14">
@@ -45943,7 +45943,7 @@
         <v>0</v>
       </c>
       <c r="N916">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="917" spans="1:14">

</xml_diff>

<commit_message>
change log and collect cards
</commit_message>
<xml_diff>
--- a/cube_cards.xlsx
+++ b/cube_cards.xlsx
@@ -4644,9 +4644,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -4654,21 +4654,6 @@
       <color theme="1"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4695,6 +4680,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
@@ -4708,16 +4700,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4742,14 +4734,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4788,6 +4772,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
@@ -4795,7 +4795,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4810,7 +4810,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4822,7 +4858,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4834,25 +4924,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4864,7 +4942,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4876,19 +4978,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4900,97 +4990,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5004,17 +5004,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5034,22 +5028,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5095,6 +5084,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -5107,10 +5107,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -5119,133 +5119,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -10237,7 +10237,7 @@
         <v>312</v>
       </c>
       <c r="C123" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>13</v>
@@ -10275,7 +10275,7 @@
         <v>314</v>
       </c>
       <c r="C124" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>13</v>
@@ -18446,7 +18446,7 @@
         <v>410</v>
       </c>
       <c r="C54">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D54" t="s">
         <v>318</v>
@@ -22059,7 +22059,7 @@
         <v>1361</v>
       </c>
       <c r="C3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>1358</v>

</xml_diff>

<commit_message>
mh2 buy a box
</commit_message>
<xml_diff>
--- a/cube_cards.xlsx
+++ b/cube_cards.xlsx
@@ -8354,9 +8354,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -8387,7 +8387,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -8402,23 +8408,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -8432,10 +8445,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -8447,16 +8485,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -8464,45 +8495,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -8518,14 +8510,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -8552,13 +8552,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8570,7 +8564,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8582,73 +8576,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8666,7 +8630,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8678,13 +8678,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8696,19 +8690,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8720,13 +8708,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8746,17 +8746,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -8768,24 +8757,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -8805,17 +8776,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -8843,16 +8808,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -8861,133 +8861,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -11656,7 +11656,7 @@
         <v>252</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50" t="s">
         <v>17</v>
@@ -13677,7 +13677,7 @@
         <v>408</v>
       </c>
       <c r="D93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E93" t="s">
         <v>313</v>
@@ -14100,7 +14100,7 @@
         <v>431</v>
       </c>
       <c r="D102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E102" t="s">
         <v>313</v>
@@ -15933,7 +15933,7 @@
         <v>571</v>
       </c>
       <c r="D141">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E141" t="s">
         <v>539</v>
@@ -18941,7 +18941,7 @@
         <v>749</v>
       </c>
       <c r="D205">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E205" t="s">
         <v>725</v>
@@ -19223,7 +19223,7 @@
         <v>772</v>
       </c>
       <c r="D211">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E211" t="s">
         <v>725</v>
@@ -23171,7 +23171,7 @@
         <v>1010</v>
       </c>
       <c r="D295">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E295" t="s">
         <v>919</v>
@@ -23829,7 +23829,7 @@
         <v>1050</v>
       </c>
       <c r="D309">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E309" t="s">
         <v>919</v>
@@ -27623,7 +27623,7 @@
         <v>1265</v>
       </c>
       <c r="D394">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E394" t="s">
         <v>1247</v>
@@ -30442,7 +30442,7 @@
         <v>1425</v>
       </c>
       <c r="D458">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E458" t="s">
         <v>1423</v>
@@ -37775,7 +37775,7 @@
         <v>1265</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" t="s">
         <v>2433</v>
@@ -44531,7 +44531,7 @@
         <v>1425</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" t="s">
         <v>2636</v>
@@ -50501,7 +50501,7 @@
         <v>1793</v>
       </c>
       <c r="D130">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E130" t="s">
         <v>17</v>
@@ -50545,7 +50545,7 @@
         <v>252</v>
       </c>
       <c r="D131">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E131" t="s">
         <v>17</v>
@@ -61184,7 +61184,7 @@
         <v>431</v>
       </c>
       <c r="D121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E121" t="s">
         <v>313</v>
@@ -61228,7 +61228,7 @@
         <v>408</v>
       </c>
       <c r="D122">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E122" t="s">
         <v>313</v>
@@ -66553,7 +66553,7 @@
         <v>571</v>
       </c>
       <c r="D120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E120" t="s">
         <v>539</v>
@@ -71920,7 +71920,7 @@
         <v>772</v>
       </c>
       <c r="D119">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E119" t="s">
         <v>725</v>
@@ -72008,7 +72008,7 @@
         <v>749</v>
       </c>
       <c r="D121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E121" t="s">
         <v>725</v>
@@ -77371,7 +77371,7 @@
         <v>1050</v>
       </c>
       <c r="D121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E121" t="s">
         <v>919</v>
@@ -77459,7 +77459,7 @@
         <v>1010</v>
       </c>
       <c r="D123">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E123" t="s">
         <v>919</v>

</xml_diff>